<commit_message>
vai começar a putaria
</commit_message>
<xml_diff>
--- a/tabelas novas/4. temporary_replacements.xlsx
+++ b/tabelas novas/4. temporary_replacements.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documentos\GitHub\project123\tabelas novas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\project123\tabelas novas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,16 +479,16 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B4:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="29.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -506,7 +506,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -515,7 +515,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -524,7 +524,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -533,7 +533,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -542,7 +542,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -551,7 +551,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -560,7 +560,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -569,7 +569,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -578,7 +578,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -587,7 +587,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -596,7 +596,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -605,7 +605,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -614,7 +614,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -623,7 +623,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -632,7 +632,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -641,52 +641,52 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
     </row>
   </sheetData>

</xml_diff>